<commit_message>
Adding ArrayType and MapType tabs to the PySparkV2.xlsx
</commit_message>
<xml_diff>
--- a/DE_Concepts.xlsx
+++ b/DE_Concepts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\Confidential\data-cloudops-natvie\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7C282BEF-2D24-4D51-838A-15D0B45A8C74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{389F7C57-4D04-4B6F-BD03-AA3EFC0DAB04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="14476" xr2:uid="{9F53CED3-BFEF-45D3-A79D-599F0C3B5EC5}"/>
   </bookViews>
@@ -1190,10 +1190,10 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1602,10 +1602,10 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>10</v>
       </c>
       <c r="C2" s="2" t="s">
@@ -1631,7 +1631,7 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A3" s="3"/>
+      <c r="A3" s="4"/>
       <c r="B3" s="2" t="s">
         <v>18</v>
       </c>
@@ -1658,8 +1658,8 @@
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A4" s="3"/>
-      <c r="B4" s="4" t="s">
+      <c r="A4" s="4"/>
+      <c r="B4" s="3" t="s">
         <v>25</v>
       </c>
       <c r="C4" s="2" t="s">
@@ -1685,7 +1685,7 @@
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A5" s="3"/>
+      <c r="A5" s="4"/>
       <c r="B5" s="2" t="s">
         <v>31</v>
       </c>
@@ -1712,7 +1712,7 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A6" s="3"/>
+      <c r="A6" s="4"/>
       <c r="B6" s="2" t="s">
         <v>37</v>
       </c>
@@ -1739,7 +1739,7 @@
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A7" s="3"/>
+      <c r="A7" s="4"/>
       <c r="B7" s="2" t="s">
         <v>43</v>
       </c>
@@ -1766,10 +1766,10 @@
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="3" t="s">
         <v>51</v>
       </c>
       <c r="C8" s="2" t="s">
@@ -1795,8 +1795,8 @@
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A9" s="3"/>
-      <c r="B9" s="4" t="s">
+      <c r="A9" s="4"/>
+      <c r="B9" s="3" t="s">
         <v>57</v>
       </c>
       <c r="C9" s="2" t="s">
@@ -1822,7 +1822,7 @@
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A10" s="3"/>
+      <c r="A10" s="4"/>
       <c r="B10" s="2" t="s">
         <v>63</v>
       </c>
@@ -1849,7 +1849,7 @@
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A11" s="3" t="s">
+      <c r="A11" s="4" t="s">
         <v>69</v>
       </c>
       <c r="B11" s="2" t="s">
@@ -1878,7 +1878,7 @@
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A12" s="3"/>
+      <c r="A12" s="4"/>
       <c r="B12" s="2" t="s">
         <v>76</v>
       </c>
@@ -1905,7 +1905,7 @@
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A13" s="3"/>
+      <c r="A13" s="4"/>
       <c r="B13" s="2" t="s">
         <v>82</v>
       </c>
@@ -1932,7 +1932,7 @@
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A14" s="3"/>
+      <c r="A14" s="4"/>
       <c r="B14" s="2" t="s">
         <v>87</v>
       </c>
@@ -1959,7 +1959,7 @@
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A15" s="3"/>
+      <c r="A15" s="4"/>
       <c r="B15" s="2" t="s">
         <v>187</v>
       </c>
@@ -1986,7 +1986,7 @@
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A16" s="3"/>
+      <c r="A16" s="4"/>
       <c r="B16" s="2" t="s">
         <v>93</v>
       </c>
@@ -2013,7 +2013,7 @@
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A17" s="3"/>
+      <c r="A17" s="4"/>
       <c r="B17" s="2" t="s">
         <v>199</v>
       </c>
@@ -2040,7 +2040,7 @@
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A18" s="3"/>
+      <c r="A18" s="4"/>
       <c r="B18" s="2" t="s">
         <v>93</v>
       </c>
@@ -2067,7 +2067,7 @@
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A19" s="3" t="s">
+      <c r="A19" s="4" t="s">
         <v>98</v>
       </c>
       <c r="B19" s="2" t="s">
@@ -2096,7 +2096,7 @@
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A20" s="3"/>
+      <c r="A20" s="4"/>
       <c r="B20" s="2" t="s">
         <v>105</v>
       </c>
@@ -2123,7 +2123,7 @@
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A21" s="3"/>
+      <c r="A21" s="4"/>
       <c r="B21" s="2" t="s">
         <v>111</v>
       </c>
@@ -2150,7 +2150,7 @@
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A22" s="3"/>
+      <c r="A22" s="4"/>
       <c r="B22" s="2" t="s">
         <v>156</v>
       </c>
@@ -2177,7 +2177,7 @@
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A23" s="3"/>
+      <c r="A23" s="4"/>
       <c r="B23" s="2" t="s">
         <v>117</v>
       </c>
@@ -2204,7 +2204,7 @@
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A24" s="3"/>
+      <c r="A24" s="4"/>
       <c r="B24" s="2" t="s">
         <v>111</v>
       </c>
@@ -2260,7 +2260,7 @@
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A26" s="3" t="s">
+      <c r="A26" s="4" t="s">
         <v>130</v>
       </c>
       <c r="B26" s="2" t="s">
@@ -2289,7 +2289,7 @@
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A27" s="3"/>
+      <c r="A27" s="4"/>
       <c r="B27" s="2" t="s">
         <v>146</v>
       </c>
@@ -2316,7 +2316,7 @@
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A28" s="3"/>
+      <c r="A28" s="4"/>
       <c r="B28" s="2" t="s">
         <v>151</v>
       </c>
@@ -2343,7 +2343,7 @@
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A29" s="3"/>
+      <c r="A29" s="4"/>
       <c r="B29" s="2" t="s">
         <v>151</v>
       </c>
@@ -2370,7 +2370,7 @@
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A30" s="3" t="s">
+      <c r="A30" s="4" t="s">
         <v>174</v>
       </c>
       <c r="B30" s="2" t="s">
@@ -2399,7 +2399,7 @@
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A31" s="3"/>
+      <c r="A31" s="4"/>
       <c r="B31" s="2" t="s">
         <v>181</v>
       </c>
@@ -2426,7 +2426,7 @@
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A32" s="3"/>
+      <c r="A32" s="4"/>
       <c r="B32" s="2" t="s">
         <v>193</v>
       </c>
@@ -2453,7 +2453,7 @@
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A33" s="3"/>
+      <c r="A33" s="4"/>
       <c r="B33" s="2" t="s">
         <v>204</v>
       </c>
@@ -2480,7 +2480,7 @@
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A34" s="3"/>
+      <c r="A34" s="4"/>
       <c r="B34" s="2" t="s">
         <v>210</v>
       </c>
@@ -2507,7 +2507,7 @@
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A35" s="3" t="s">
+      <c r="A35" s="4" t="s">
         <v>162</v>
       </c>
       <c r="B35" s="2" t="s">
@@ -2536,7 +2536,7 @@
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A36" s="3"/>
+      <c r="A36" s="4"/>
       <c r="B36" s="2" t="s">
         <v>169</v>
       </c>

</xml_diff>

<commit_message>
Added DeltaLake+Hudi+Iceberg details in DE_Concepts.xlsx
</commit_message>
<xml_diff>
--- a/DE_Concepts.xlsx
+++ b/DE_Concepts.xlsx
@@ -8,20 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\Confidential\data-cloudops-natvie\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{389F7C57-4D04-4B6F-BD03-AA3EFC0DAB04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{784E593B-F910-48BC-8BDC-14D594087B25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="14476" xr2:uid="{9F53CED3-BFEF-45D3-A79D-599F0C3B5EC5}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="14476" activeTab="1" xr2:uid="{9F53CED3-BFEF-45D3-A79D-599F0C3B5EC5}"/>
   </bookViews>
   <sheets>
     <sheet name="parquet" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
+    <sheet name="DeltaLake" sheetId="4" r:id="rId2"/>
+    <sheet name="DeltaLake vs Hudi vs Iceberg" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="601" uniqueCount="474">
   <si>
     <t>Category</t>
   </si>
@@ -666,6 +667,869 @@
   </si>
   <si>
     <t>Processing a petabyte-scale dataset in Spark.</t>
+  </si>
+  <si>
+    <t>Feature/Aspect</t>
+  </si>
+  <si>
+    <t>Delta Lake</t>
+  </si>
+  <si>
+    <t>Apache Hudi</t>
+  </si>
+  <si>
+    <t>Apache Iceberg</t>
+  </si>
+  <si>
+    <t>Primary Use Case</t>
+  </si>
+  <si>
+    <t>Batch and streaming data processing</t>
+  </si>
+  <si>
+    <t>Real-time data ingestion and upserts</t>
+  </si>
+  <si>
+    <t>Large-scale, immutable analytical datasets</t>
+  </si>
+  <si>
+    <t>Data Format</t>
+  </si>
+  <si>
+    <t>Parquet</t>
+  </si>
+  <si>
+    <t>Parquet, ORC, Avro</t>
+  </si>
+  <si>
+    <t>Versioning</t>
+  </si>
+  <si>
+    <t>Supports versioned tables</t>
+  </si>
+  <si>
+    <t>ACID Transactions</t>
+  </si>
+  <si>
+    <t>Yes (via transaction logs)</t>
+  </si>
+  <si>
+    <t>Yes (via timeline and commit protocols)</t>
+  </si>
+  <si>
+    <t>Yes (via snapshot isolation)</t>
+  </si>
+  <si>
+    <t>Schema Evolution</t>
+  </si>
+  <si>
+    <t>Supported (with schema validation)</t>
+  </si>
+  <si>
+    <t>Partitioning</t>
+  </si>
+  <si>
+    <t>Partition pruning</t>
+  </si>
+  <si>
+    <t>Supports primary key-based updates and deletes</t>
+  </si>
+  <si>
+    <t>Automatic partitioning (no manual management)</t>
+  </si>
+  <si>
+    <t>Indexing</t>
+  </si>
+  <si>
+    <t>No native indexing</t>
+  </si>
+  <si>
+    <t>Built-in indexing for faster queries</t>
+  </si>
+  <si>
+    <t>Compaction</t>
+  </si>
+  <si>
+    <t>Not a primary feature</t>
+  </si>
+  <si>
+    <t>Supports asynchronous and inline compaction</t>
+  </si>
+  <si>
+    <t>Streaming Support</t>
+  </si>
+  <si>
+    <t>Supports streaming writes and reads</t>
+  </si>
+  <si>
+    <t>Designed for streaming ingestion and upserts</t>
+  </si>
+  <si>
+    <t>Primarily batch-oriented</t>
+  </si>
+  <si>
+    <t>Concurrency Control</t>
+  </si>
+  <si>
+    <t>Optimistic concurrency control</t>
+  </si>
+  <si>
+    <t>Snapshot-based isolation</t>
+  </si>
+  <si>
+    <t>Merge-on-Read vs Copy-on-Write</t>
+  </si>
+  <si>
+    <t>Primarily Copy-on-Write</t>
+  </si>
+  <si>
+    <t>Supports both (configurable per table)</t>
+  </si>
+  <si>
+    <t>Checkpointing</t>
+  </si>
+  <si>
+    <t>Built-in via transaction log</t>
+  </si>
+  <si>
+    <t>Built-in for incremental processing</t>
+  </si>
+  <si>
+    <t>Managed via snapshots</t>
+  </si>
+  <si>
+    <t>Data Layout Optimization</t>
+  </si>
+  <si>
+    <t>Z-order clustering</t>
+  </si>
+  <si>
+    <t>Clustering and file compaction</t>
+  </si>
+  <si>
+    <t>Automatic partition evolution</t>
+  </si>
+  <si>
+    <t>Query Performance Enhancements</t>
+  </si>
+  <si>
+    <t>Bloom filters, column pruning, and indexing</t>
+  </si>
+  <si>
+    <t>Hidden partitioning, metadata pruning</t>
+  </si>
+  <si>
+    <t>Integration with Query Engines</t>
+  </si>
+  <si>
+    <t>Presto, Hive, Spark, Flink, Trino</t>
+  </si>
+  <si>
+    <t>Metadata Management</t>
+  </si>
+  <si>
+    <t>Transaction log</t>
+  </si>
+  <si>
+    <t>Timeline server</t>
+  </si>
+  <si>
+    <t>Metadata tree with snapshots</t>
+  </si>
+  <si>
+    <t>Time Travel</t>
+  </si>
+  <si>
+    <t>Supported</t>
+  </si>
+  <si>
+    <t>Support for Object Stores</t>
+  </si>
+  <si>
+    <t>S3, GCS, Azure, HDFS</t>
+  </si>
+  <si>
+    <t>Data Deletion/Retention</t>
+  </si>
+  <si>
+    <t>Supports deletes but less optimized</t>
+  </si>
+  <si>
+    <t>Optimized for GDPR compliance (deletes)</t>
+  </si>
+  <si>
+    <t>Supports deletes with snapshot expiration</t>
+  </si>
+  <si>
+    <t>Data Governance Features</t>
+  </si>
+  <si>
+    <t>Limited native support</t>
+  </si>
+  <si>
+    <t>Built-in metadata tracking and auditing</t>
+  </si>
+  <si>
+    <t>Cost Optimization</t>
+  </si>
+  <si>
+    <t>Focused on reducing I/O costs</t>
+  </si>
+  <si>
+    <t>Incremental processing reduces storage costs</t>
+  </si>
+  <si>
+    <t>Optimized for query performance and cost</t>
+  </si>
+  <si>
+    <t>Catalog Integration</t>
+  </si>
+  <si>
+    <t>Hive Metastore, Glue Catalog</t>
+  </si>
+  <si>
+    <t>Hive Metastore, Glue Catalog, etc.</t>
+  </si>
+  <si>
+    <t>Hive Metastore, Glue Catalog, Nessie</t>
+  </si>
+  <si>
+    <t>Compaction Granularity</t>
+  </si>
+  <si>
+    <t>Configurable (file-level or partition-level)</t>
+  </si>
+  <si>
+    <t>Managed at the snapshot level</t>
+  </si>
+  <si>
+    <t>Support for CDC (Change Data Capture)</t>
+  </si>
+  <si>
+    <t>Limited support</t>
+  </si>
+  <si>
+    <t>Native support</t>
+  </si>
+  <si>
+    <t>Write Amplification</t>
+  </si>
+  <si>
+    <t>Higher due to Copy-on-Write</t>
+  </si>
+  <si>
+    <t>Reduced via incremental updates</t>
+  </si>
+  <si>
+    <t>Moderate due to snapshot isolation</t>
+  </si>
+  <si>
+    <t>Read Amplification</t>
+  </si>
+  <si>
+    <t>Reduced via indexing and pruning</t>
+  </si>
+  <si>
+    <t>Reduced via hidden partitioning</t>
+  </si>
+  <si>
+    <t>Ecosystem Maturity</t>
+  </si>
+  <si>
+    <t>Strong in Spark-based workflows</t>
+  </si>
+  <si>
+    <t>Strong in real-time and streaming use cases</t>
+  </si>
+  <si>
+    <t>Growing with analytical use cases</t>
+  </si>
+  <si>
+    <t>File Format Evolution</t>
+  </si>
+  <si>
+    <t>Limited</t>
+  </si>
+  <si>
+    <t>Supports evolving file formats</t>
+  </si>
+  <si>
+    <t>Governance and Lineage</t>
+  </si>
+  <si>
+    <t>Stronger focus on governance and lineage</t>
+  </si>
+  <si>
+    <t>Community Governance</t>
+  </si>
+  <si>
+    <t>Databricks-led</t>
+  </si>
+  <si>
+    <t>Apache Software Foundation</t>
+  </si>
+  <si>
+    <t>Optimized for batch and streaming</t>
+  </si>
+  <si>
+    <t>Optimized for incremental processing</t>
+  </si>
+  <si>
+    <t>Optimized for large-scale analytical queries</t>
+  </si>
+  <si>
+    <t>Practical Use Cases</t>
+  </si>
+  <si>
+    <t>ETL pipelines, machine learning workflows, and batch processing</t>
+  </si>
+  <si>
+    <t>Real-time fraud detection, IoT data ingestion, and GDPR compliance</t>
+  </si>
+  <si>
+    <t>Data warehousing, large-scale analytics, and immutable data lakes</t>
+  </si>
+  <si>
+    <t>Ecosystem Integration</t>
+  </si>
+  <si>
+    <t>Tight integration with Spark and Databricks</t>
+  </si>
+  <si>
+    <t>Works with Spark, Flink, Hive, Presto, Trino</t>
+  </si>
+  <si>
+    <t>Works with Spark, Flink, Hive, Presto, Trino, and Nessie</t>
+  </si>
+  <si>
+    <t>Quantitative Metrics</t>
+  </si>
+  <si>
+    <t>Latency: Low for batch; moderate for streaming. _x000D_
+Throughput: High batch throughput. _x000D_
+Storage Efficiency: Moderate due to Copy-on-Write</t>
+  </si>
+  <si>
+    <t>Latency: Low for real-time ingestion. _x000D_
+Throughput: High for incremental updates. _x000D_
+Storage Efficiency: High due to Merge-on-Read</t>
+  </si>
+  <si>
+    <t>Latency: Low for analytical queries. _x000D_
+Throughput: High for large-scale queries. _x000D_
+Storage Efficiency: High due to snapshot isolation</t>
+  </si>
+  <si>
+    <t>Real-World Examples</t>
+  </si>
+  <si>
+    <t>Used by Databricks customers for ETL and ML workflows. _x000D_
+Widely adopted in financial services and retail</t>
+  </si>
+  <si>
+    <t>Uber uses Hudi for real-time trip data processing. _x000D_
+Used in IoT platforms for incremental updates</t>
+  </si>
+  <si>
+    <t>Netflix uses Iceberg for analytical workloads. _x000D_
+AWS and Snowflake support Iceberg for data warehousing</t>
+  </si>
+  <si>
+    <t>Future Roadmap or Feature Gaps</t>
+  </si>
+  <si>
+    <t>Focus on improving governance and indexing. _x000D_
+Limited support for non-Spark environments</t>
+  </si>
+  <si>
+    <t>Expanding Flink integration and scaling capabilities. _x000D_
+Limited governance features compared to Iceberg</t>
+  </si>
+  <si>
+    <t>Improving CDC support and streaming capabilities. _x000D_
+Limited real-time ingestion support</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Delta Lake</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">:
+  - Offers strong support for both batch and streaming use cases.
+  - Backed by Databricks, with tight integration with Spark.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Apache Hudi</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">:
+  - Best for real-time use cases with frequent updates and upserts.
+  - Includes built-in indexing and compaction mechanisms for efficient storage and query performance.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Apache Iceberg</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>:
+  - Designed for large-scale analytical workloads with a focus on immutability and governance.
+  - Hidden partitioning simplifies user experience.
+How to Choose:
+  - Choose Apache Hudi if you need real-time ingestion, upserts, and streaming capabilities.
+  - Choose Delta Lake if you are heavily reliant on Spark and need robust support for both batch and streaming pipelines.
+  - Choose Apache Iceberg if you prioritize query performance at scale, governance, and analytical workloads.</t>
+    </r>
+  </si>
+  <si>
+    <t>Use Case</t>
+  </si>
+  <si>
+    <t>Challenges Addressed</t>
+  </si>
+  <si>
+    <t>Benefit</t>
+  </si>
+  <si>
+    <t>Data Reliability</t>
+  </si>
+  <si>
+    <t>Ensures data consistency and reliability even in distributed environments.</t>
+  </si>
+  <si>
+    <t>Multiple users writing to the same Delta Table will have consistent results without data corruption.</t>
+  </si>
+  <si>
+    <t>Ensuring reliable data pipelines for ETL (Extract, Transform, Load) workflows.</t>
+  </si>
+  <si>
+    <t>Prevents partial writes or data corruption.</t>
+  </si>
+  <si>
+    <t>Guarantees consistent and reliable data operations.</t>
+  </si>
+  <si>
+    <t>Data Quality</t>
+  </si>
+  <si>
+    <t>Schema Enforcement</t>
+  </si>
+  <si>
+    <t>Prevents invalid data by enforcing a predefined schema during writes.</t>
+  </si>
+  <si>
+    <t>A table with a schema expecting an integer column will reject non-integer values.</t>
+  </si>
+  <si>
+    <t>Maintaining clean and consistent data for analytics and machine learning tasks.</t>
+  </si>
+  <si>
+    <t>Prevents inconsistent or invalid data.</t>
+  </si>
+  <si>
+    <t>Ensures data integrity and reliability.</t>
+  </si>
+  <si>
+    <t>Allows updates to the schema without breaking existing pipelines.</t>
+  </si>
+  <si>
+    <t>Adding a new column to a Delta Table without rewriting the entire dataset.</t>
+  </si>
+  <si>
+    <t>Adapting to changing business requirements or evolving datasets over time.</t>
+  </si>
+  <si>
+    <t>Avoids manual intervention for schema changes.</t>
+  </si>
+  <si>
+    <t>Simplifies handling of evolving data schemas.</t>
+  </si>
+  <si>
+    <t>Data Versioning</t>
+  </si>
+  <si>
+    <t>Enables querying historical versions of data using timestamps or version IDs.</t>
+  </si>
+  <si>
+    <t>Querying a Delta Table as it existed 7 days ago: df.option("timestampAsOf", "2023-10-01").load()</t>
+  </si>
+  <si>
+    <t>Debugging issues, auditing historical data, or reproducing machine learning experiments.</t>
+  </si>
+  <si>
+    <t>Lack of historical data tracking.</t>
+  </si>
+  <si>
+    <t>Provides full data traceability and reproducibility.</t>
+  </si>
+  <si>
+    <t>Performance Optimization</t>
+  </si>
+  <si>
+    <t>Data Compaction</t>
+  </si>
+  <si>
+    <t>Combines small files into larger ones to improve query performance.</t>
+  </si>
+  <si>
+    <t>Merging 1,000 small Parquet files into 10 larger files for faster reads.</t>
+  </si>
+  <si>
+    <t>Optimizing storage and query performance in large-scale data lakes.</t>
+  </si>
+  <si>
+    <t>Inefficient storage and slow queries.</t>
+  </si>
+  <si>
+    <t>Improves query speed and reduces storage overhead.</t>
+  </si>
+  <si>
+    <t>Scalable Metadata Handling</t>
+  </si>
+  <si>
+    <t>Efficiently manages metadata for large datasets, ensuring faster queries.</t>
+  </si>
+  <si>
+    <t>Delta Lake can handle millions of partitions without performance degradation.</t>
+  </si>
+  <si>
+    <t>Querying petabyte-scale datasets without slowdowns.</t>
+  </si>
+  <si>
+    <t>Slow metadata operations in large datasets.</t>
+  </si>
+  <si>
+    <t>Enables fast queries on large-scale data lakes.</t>
+  </si>
+  <si>
+    <t>Z-Ordering</t>
+  </si>
+  <si>
+    <t>Optimizes data layout by co-locating related data for faster queries.</t>
+  </si>
+  <si>
+    <t>Sorting data by a frequently queried column (e.g., date) to speed up query performance.</t>
+  </si>
+  <si>
+    <t>Improving query performance for analytical workloads with large datasets.</t>
+  </si>
+  <si>
+    <t>Unoptimized data layout for queries.</t>
+  </si>
+  <si>
+    <t>Reduces query latency for frequently accessed data.</t>
+  </si>
+  <si>
+    <t>Automatically skips irrelevant data during queries for improved performance.</t>
+  </si>
+  <si>
+    <t>Querying a Delta Table with filters automatically excludes non-matching partitions.</t>
+  </si>
+  <si>
+    <t>Reducing query times for large datasets by avoiding unnecessary data scans.</t>
+  </si>
+  <si>
+    <t>Scanning irrelevant data during queries.</t>
+  </si>
+  <si>
+    <t>Accelerates query performance by skipping unnecessary data.</t>
+  </si>
+  <si>
+    <t>Unified Processing</t>
+  </si>
+  <si>
+    <t>Batch and Streaming</t>
+  </si>
+  <si>
+    <t>Supports both batch and streaming data processing in a single framework.</t>
+  </si>
+  <si>
+    <t>Ingesting real-time streaming data while running batch queries on the same Delta Table.</t>
+  </si>
+  <si>
+    <t>Building real-time dashboards and analytics pipelines.</t>
+  </si>
+  <si>
+    <t>Separate systems for batch and streaming.</t>
+  </si>
+  <si>
+    <t>Simplifies architecture with unified processing.</t>
+  </si>
+  <si>
+    <t>Change Data Capture (CDC)</t>
+  </si>
+  <si>
+    <t>Tracks and captures changes (inserts, updates, deletes) in Delta Tables.</t>
+  </si>
+  <si>
+    <t>Capturing only the updated rows from a Delta Table for downstream processing.</t>
+  </si>
+  <si>
+    <t>Propagating changes in real-time to downstream systems or applications.</t>
+  </si>
+  <si>
+    <t>Difficulty in tracking incremental changes.</t>
+  </si>
+  <si>
+    <t>Enables real-time updates for downstream systems.</t>
+  </si>
+  <si>
+    <t>Data Governance</t>
+  </si>
+  <si>
+    <t>Data Lineage</t>
+  </si>
+  <si>
+    <t>Tracks all changes made to the data for full auditability.</t>
+  </si>
+  <si>
+    <t>Viewing the history of a Delta Table using DESCRIBE HISTORY delta_table_path.</t>
+  </si>
+  <si>
+    <t>Meeting regulatory compliance and auditing requirements for sensitive datasets.</t>
+  </si>
+  <si>
+    <t>Lack of traceability in data changes.</t>
+  </si>
+  <si>
+    <t>Ensures accountability and compliance.</t>
+  </si>
+  <si>
+    <t>Retention Policies</t>
+  </si>
+  <si>
+    <t>Allows automatic cleanup of old data based on retention rules.</t>
+  </si>
+  <si>
+    <t>Configuring a table to retain only the last 30 days of data.</t>
+  </si>
+  <si>
+    <t>Managing storage costs and ensuring compliance with data retention policies.</t>
+  </si>
+  <si>
+    <t>Accumulation of outdated data.</t>
+  </si>
+  <si>
+    <t>Reduces storage costs and enforces data lifecycle policies.</t>
+  </si>
+  <si>
+    <t>Integration</t>
+  </si>
+  <si>
+    <t>Delta Table</t>
+  </si>
+  <si>
+    <t>A dataset stored in Delta Lake format, queryable via Spark SQL.</t>
+  </si>
+  <si>
+    <t>Creating a Delta Table: df.write.format("delta").save("/path/to/delta-table")</t>
+  </si>
+  <si>
+    <t>Storing structured or semi-structured data for analysis and reporting.</t>
+  </si>
+  <si>
+    <t>Lack of format compatibility with analytics tools.</t>
+  </si>
+  <si>
+    <t>Provides a flexible and queryable data format.</t>
+  </si>
+  <si>
+    <t>Flexibility</t>
+  </si>
+  <si>
+    <t>Supports dynamic changes to the table's schema without manual intervention.</t>
+  </si>
+  <si>
+    <t>Automatically adding a new column when new data includes it.</t>
+  </si>
+  <si>
+    <t>Adapting to unstructured or semi-structured data sources, such as JSON or IoT data streams.</t>
+  </si>
+  <si>
+    <t>Difficulty in handling evolving data formats.</t>
+  </si>
+  <si>
+    <t>Simplifies schema management for dynamic datasets.</t>
+  </si>
+  <si>
+    <t>Historical Insights</t>
+  </si>
+  <si>
+    <t>Audit Logs</t>
+  </si>
+  <si>
+    <t>Maintains a detailed log of all operations (e.g., inserts, updates, deletes).</t>
+  </si>
+  <si>
+    <t>Retrieving a log of all changes made to a table for auditing purposes.</t>
+  </si>
+  <si>
+    <t>Ensuring accountability and traceability for sensitive or regulated datasets.</t>
+  </si>
+  <si>
+    <t>Lack of visibility into data operations.</t>
+  </si>
+  <si>
+    <t>Provides full transparency for auditing purposes.</t>
+  </si>
+  <si>
+    <t>Data Sharing</t>
+  </si>
+  <si>
+    <t>Delta Sharing</t>
+  </si>
+  <si>
+    <t>Enables secure, real-time data sharing across organizations.</t>
+  </si>
+  <si>
+    <t>Sharing a Delta Table with a partner organization without duplicating the data.</t>
+  </si>
+  <si>
+    <t>Collaborating with external teams or partners on shared datasets securely and efficiently.</t>
+  </si>
+  <si>
+    <t>Difficulty in securely sharing large datasets.</t>
+  </si>
+  <si>
+    <t>Facilitates secure and efficient data collaboration.</t>
+  </si>
+  <si>
+    <t>Error Handling</t>
+  </si>
+  <si>
+    <t>Upserts and Deletes</t>
+  </si>
+  <si>
+    <t>Supports updates and deletes directly on Delta Tables.</t>
+  </si>
+  <si>
+    <t>Updating specific rows in a Delta Table using SQL: MERGE INTO delta_table USING updates ...</t>
+  </si>
+  <si>
+    <t>Handling late-arriving data or correcting errors in already-ingested data.</t>
+  </si>
+  <si>
+    <t>Difficulty in modifying existing data.</t>
+  </si>
+  <si>
+    <t>Simplifies handling of late-arriving or incorrect data.</t>
+  </si>
+  <si>
+    <t>Concurrency Handling</t>
+  </si>
+  <si>
+    <t>Optimistic Concurrency Control</t>
+  </si>
+  <si>
+    <t>Ensures multiple users can write to the same table without conflicts.</t>
+  </si>
+  <si>
+    <t>Two users updating different parts of the table will not interfere with each other.</t>
+  </si>
+  <si>
+    <t>Supporting collaborative data pipelines with multiple contributors.</t>
+  </si>
+  <si>
+    <t>Conflicts during concurrent data writes.</t>
+  </si>
+  <si>
+    <t>Enables safe and conflict-free concurrent operations.</t>
+  </si>
+  <si>
+    <t>Advanced Features</t>
+  </si>
+  <si>
+    <t>Incremental Data Loading</t>
+  </si>
+  <si>
+    <t>Supports loading only new or changed data into Delta Tables.</t>
+  </si>
+  <si>
+    <t>Using MERGE to load only the latest changes into a Delta Table.</t>
+  </si>
+  <si>
+    <t>Building efficient data pipelines for real-time or near-real-time processing.</t>
+  </si>
+  <si>
+    <t>Reprocessing entire datasets for small updates.</t>
+  </si>
+  <si>
+    <t>Saves time and resources by processing only new data.</t>
+  </si>
+  <si>
+    <t>Caching</t>
+  </si>
+  <si>
+    <t>Speeds up queries by caching frequently accessed data in memory.</t>
+  </si>
+  <si>
+    <t>Using Spark's cache() API to store Delta Table data in memory for faster reads.</t>
+  </si>
+  <si>
+    <t>Improving performance for frequently queried datasets in analytics workflows.</t>
+  </si>
+  <si>
+    <t>Slow queries on frequently accessed data.</t>
+  </si>
+  <si>
+    <t>Improves query speed for repeated access patterns.</t>
+  </si>
+  <si>
+    <t>Allows splitting data into partitions for efficient storage and querying.</t>
+  </si>
+  <si>
+    <t>Partitioning a table by year or region for faster queries on those dimensions.</t>
+  </si>
+  <si>
+    <t>Optimizing storage and query performance for large-scale datasets.</t>
+  </si>
+  <si>
+    <t>Enables faster queries and better storage management.</t>
   </si>
 </sst>
 </file>
@@ -816,7 +1680,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="35">
+  <fills count="36">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1008,8 +1872,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="11">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -1139,6 +2009,126 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1184,7 +2174,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1192,6 +2182,72 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="35" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1554,9 +2610,9 @@
   </sheetPr>
   <dimension ref="A1:I37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C15" sqref="C15"/>
+      <selection pane="bottomLeft" activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1602,7 +2658,7 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="5" t="s">
         <v>9</v>
       </c>
       <c r="B2" s="3" t="s">
@@ -1631,7 +2687,7 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A3" s="4"/>
+      <c r="A3" s="5"/>
       <c r="B3" s="2" t="s">
         <v>18</v>
       </c>
@@ -1658,7 +2714,7 @@
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A4" s="4"/>
+      <c r="A4" s="5"/>
       <c r="B4" s="3" t="s">
         <v>25</v>
       </c>
@@ -1685,7 +2741,7 @@
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A5" s="4"/>
+      <c r="A5" s="5"/>
       <c r="B5" s="2" t="s">
         <v>31</v>
       </c>
@@ -1712,7 +2768,7 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A6" s="4"/>
+      <c r="A6" s="5"/>
       <c r="B6" s="2" t="s">
         <v>37</v>
       </c>
@@ -1739,7 +2795,7 @@
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A7" s="4"/>
+      <c r="A7" s="5"/>
       <c r="B7" s="2" t="s">
         <v>43</v>
       </c>
@@ -1766,7 +2822,7 @@
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="5" t="s">
         <v>50</v>
       </c>
       <c r="B8" s="3" t="s">
@@ -1795,7 +2851,7 @@
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A9" s="4"/>
+      <c r="A9" s="5"/>
       <c r="B9" s="3" t="s">
         <v>57</v>
       </c>
@@ -1822,7 +2878,7 @@
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A10" s="4"/>
+      <c r="A10" s="5"/>
       <c r="B10" s="2" t="s">
         <v>63</v>
       </c>
@@ -1849,7 +2905,7 @@
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A11" s="4" t="s">
+      <c r="A11" s="5" t="s">
         <v>69</v>
       </c>
       <c r="B11" s="2" t="s">
@@ -1878,7 +2934,7 @@
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A12" s="4"/>
+      <c r="A12" s="5"/>
       <c r="B12" s="2" t="s">
         <v>76</v>
       </c>
@@ -1905,7 +2961,7 @@
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A13" s="4"/>
+      <c r="A13" s="5"/>
       <c r="B13" s="2" t="s">
         <v>82</v>
       </c>
@@ -1932,7 +2988,7 @@
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A14" s="4"/>
+      <c r="A14" s="5"/>
       <c r="B14" s="2" t="s">
         <v>87</v>
       </c>
@@ -1959,7 +3015,7 @@
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A15" s="4"/>
+      <c r="A15" s="5"/>
       <c r="B15" s="2" t="s">
         <v>187</v>
       </c>
@@ -1986,7 +3042,7 @@
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A16" s="4"/>
+      <c r="A16" s="5"/>
       <c r="B16" s="2" t="s">
         <v>93</v>
       </c>
@@ -2013,7 +3069,7 @@
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A17" s="4"/>
+      <c r="A17" s="5"/>
       <c r="B17" s="2" t="s">
         <v>199</v>
       </c>
@@ -2040,7 +3096,7 @@
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A18" s="4"/>
+      <c r="A18" s="5"/>
       <c r="B18" s="2" t="s">
         <v>93</v>
       </c>
@@ -2067,7 +3123,7 @@
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A19" s="4" t="s">
+      <c r="A19" s="5" t="s">
         <v>98</v>
       </c>
       <c r="B19" s="2" t="s">
@@ -2096,7 +3152,7 @@
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A20" s="4"/>
+      <c r="A20" s="5"/>
       <c r="B20" s="2" t="s">
         <v>105</v>
       </c>
@@ -2123,7 +3179,7 @@
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A21" s="4"/>
+      <c r="A21" s="5"/>
       <c r="B21" s="2" t="s">
         <v>111</v>
       </c>
@@ -2150,7 +3206,7 @@
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A22" s="4"/>
+      <c r="A22" s="5"/>
       <c r="B22" s="2" t="s">
         <v>156</v>
       </c>
@@ -2177,7 +3233,7 @@
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A23" s="4"/>
+      <c r="A23" s="5"/>
       <c r="B23" s="2" t="s">
         <v>117</v>
       </c>
@@ -2204,7 +3260,7 @@
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A24" s="4"/>
+      <c r="A24" s="5"/>
       <c r="B24" s="2" t="s">
         <v>111</v>
       </c>
@@ -2260,7 +3316,7 @@
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A26" s="4" t="s">
+      <c r="A26" s="5" t="s">
         <v>130</v>
       </c>
       <c r="B26" s="2" t="s">
@@ -2289,7 +3345,7 @@
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A27" s="4"/>
+      <c r="A27" s="5"/>
       <c r="B27" s="2" t="s">
         <v>146</v>
       </c>
@@ -2316,7 +3372,7 @@
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A28" s="4"/>
+      <c r="A28" s="5"/>
       <c r="B28" s="2" t="s">
         <v>151</v>
       </c>
@@ -2343,7 +3399,7 @@
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A29" s="4"/>
+      <c r="A29" s="5"/>
       <c r="B29" s="2" t="s">
         <v>151</v>
       </c>
@@ -2370,7 +3426,7 @@
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A30" s="4" t="s">
+      <c r="A30" s="5" t="s">
         <v>174</v>
       </c>
       <c r="B30" s="2" t="s">
@@ -2399,7 +3455,7 @@
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A31" s="4"/>
+      <c r="A31" s="5"/>
       <c r="B31" s="2" t="s">
         <v>181</v>
       </c>
@@ -2426,7 +3482,7 @@
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A32" s="4"/>
+      <c r="A32" s="5"/>
       <c r="B32" s="2" t="s">
         <v>193</v>
       </c>
@@ -2453,7 +3509,7 @@
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A33" s="4"/>
+      <c r="A33" s="5"/>
       <c r="B33" s="2" t="s">
         <v>204</v>
       </c>
@@ -2480,7 +3536,7 @@
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A34" s="4"/>
+      <c r="A34" s="5"/>
       <c r="B34" s="2" t="s">
         <v>210</v>
       </c>
@@ -2507,7 +3563,7 @@
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A35" s="4" t="s">
+      <c r="A35" s="5" t="s">
         <v>162</v>
       </c>
       <c r="B35" s="2" t="s">
@@ -2536,7 +3592,7 @@
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A36" s="4"/>
+      <c r="A36" s="5"/>
       <c r="B36" s="2" t="s">
         <v>169</v>
       </c>
@@ -2606,13 +3662,1178 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC9EE76A-8F76-40BA-A1FA-AC82BB9FFA32}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E55E35B-AA68-42D7-B709-277C39D4CDEB}">
+  <sheetPr>
+    <tabColor theme="4" tint="0.39997558519241921"/>
+  </sheetPr>
+  <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20:A22"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.53125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="63.19921875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="79.796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="74.19921875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="39.46484375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="49.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="15" x14ac:dyDescent="0.45">
+      <c r="A1" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="17" t="s">
+        <v>339</v>
+      </c>
+      <c r="F1" s="17" t="s">
+        <v>340</v>
+      </c>
+      <c r="G1" s="18" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A2" s="19" t="s">
+        <v>342</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>228</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>343</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>344</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>345</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>346</v>
+      </c>
+      <c r="G2" s="20" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3" s="10" t="s">
+        <v>348</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>349</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>350</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>351</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>352</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>353</v>
+      </c>
+      <c r="G3" s="20" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A4" s="10"/>
+      <c r="B4" s="4" t="s">
+        <v>232</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>355</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>356</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>357</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>358</v>
+      </c>
+      <c r="G4" s="20" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A5" s="19" t="s">
+        <v>360</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>271</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>361</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>362</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>363</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>364</v>
+      </c>
+      <c r="G5" s="20" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A6" s="10" t="s">
+        <v>366</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>367</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>368</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>369</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>370</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>371</v>
+      </c>
+      <c r="G6" s="20" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A7" s="10"/>
+      <c r="B7" s="4" t="s">
+        <v>373</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>374</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>375</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>376</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>377</v>
+      </c>
+      <c r="G7" s="20" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A8" s="10"/>
+      <c r="B8" s="4" t="s">
+        <v>379</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>380</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>381</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>382</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>383</v>
+      </c>
+      <c r="G8" s="20" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A9" s="10"/>
+      <c r="B9" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>385</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>386</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>387</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>388</v>
+      </c>
+      <c r="G9" s="20" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A10" s="10" t="s">
+        <v>390</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>391</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>392</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>393</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>394</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>395</v>
+      </c>
+      <c r="G10" s="20" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A11" s="10"/>
+      <c r="B11" s="4" t="s">
+        <v>397</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>398</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>399</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>400</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>401</v>
+      </c>
+      <c r="G11" s="20" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A12" s="10" t="s">
+        <v>403</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>404</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>405</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>406</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>407</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>408</v>
+      </c>
+      <c r="G12" s="20" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A13" s="10"/>
+      <c r="B13" s="4" t="s">
+        <v>410</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>411</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>413</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>414</v>
+      </c>
+      <c r="G13" s="20" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A14" s="19" t="s">
+        <v>416</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>418</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>419</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>420</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>421</v>
+      </c>
+      <c r="G14" s="20" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A15" s="19" t="s">
+        <v>423</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>232</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>424</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>425</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>426</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>427</v>
+      </c>
+      <c r="G15" s="20" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A16" s="19" t="s">
+        <v>429</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>430</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>431</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>432</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>433</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>434</v>
+      </c>
+      <c r="G16" s="20" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A17" s="19" t="s">
+        <v>436</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>437</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>438</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>439</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>440</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>441</v>
+      </c>
+      <c r="G17" s="20" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A18" s="19" t="s">
+        <v>443</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>444</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>445</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>446</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>447</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>448</v>
+      </c>
+      <c r="G18" s="20" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A19" s="19" t="s">
+        <v>450</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>451</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>452</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>453</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>454</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>455</v>
+      </c>
+      <c r="G19" s="20" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A20" s="10" t="s">
+        <v>457</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>458</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>459</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>460</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>461</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>462</v>
+      </c>
+      <c r="G20" s="20" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A21" s="10"/>
+      <c r="B21" s="4" t="s">
+        <v>464</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>465</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>466</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>467</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>468</v>
+      </c>
+      <c r="G21" s="20" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A22" s="12"/>
+      <c r="B22" s="25" t="s">
+        <v>234</v>
+      </c>
+      <c r="C22" s="25" t="s">
+        <v>470</v>
+      </c>
+      <c r="D22" s="25" t="s">
+        <v>471</v>
+      </c>
+      <c r="E22" s="25" t="s">
+        <v>472</v>
+      </c>
+      <c r="F22" s="25" t="s">
+        <v>371</v>
+      </c>
+      <c r="G22" s="26" t="s">
+        <v>473</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="A6:A9"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="A20:A22"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB745402-F3FA-428E-9A91-7B127D6E3D80}">
+  <sheetPr>
+    <tabColor theme="7" tint="0.59999389629810485"/>
+  </sheetPr>
+  <dimension ref="A1:D59"/>
+  <sheetViews>
+    <sheetView topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="32" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="52.06640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="54.86328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="53.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="15" x14ac:dyDescent="0.45">
+      <c r="A1" s="15" t="s">
+        <v>215</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>216</v>
+      </c>
+      <c r="C1" s="17" t="s">
+        <v>217</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A2" s="19" t="s">
+        <v>219</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>221</v>
+      </c>
+      <c r="D2" s="20" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A3" s="19" t="s">
+        <v>223</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>225</v>
+      </c>
+      <c r="D3" s="20" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A4" s="19" t="s">
+        <v>226</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>227</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>227</v>
+      </c>
+      <c r="D4" s="20" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A5" s="19" t="s">
+        <v>228</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>229</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>230</v>
+      </c>
+      <c r="D5" s="20" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A6" s="19" t="s">
+        <v>232</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>233</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>233</v>
+      </c>
+      <c r="D6" s="20" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A7" s="19" t="s">
+        <v>234</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>235</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>236</v>
+      </c>
+      <c r="D7" s="20" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A8" s="19" t="s">
+        <v>238</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>239</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>240</v>
+      </c>
+      <c r="D8" s="20" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A9" s="19" t="s">
+        <v>241</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>242</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>243</v>
+      </c>
+      <c r="D9" s="20" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A10" s="19" t="s">
+        <v>244</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>245</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>246</v>
+      </c>
+      <c r="D10" s="20" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A11" s="19" t="s">
+        <v>248</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>249</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>249</v>
+      </c>
+      <c r="D11" s="20" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A12" s="19" t="s">
+        <v>251</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>252</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>253</v>
+      </c>
+      <c r="D12" s="20" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A13" s="19" t="s">
+        <v>254</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>255</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>256</v>
+      </c>
+      <c r="D13" s="20" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A14" s="19" t="s">
+        <v>258</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>259</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>260</v>
+      </c>
+      <c r="D14" s="20" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A15" s="19" t="s">
+        <v>262</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>259</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>263</v>
+      </c>
+      <c r="D15" s="20" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A16" s="19" t="s">
+        <v>265</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>266</v>
+      </c>
+      <c r="D16" s="20" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A17" s="19" t="s">
+        <v>267</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>268</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>269</v>
+      </c>
+      <c r="D17" s="20" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A18" s="19" t="s">
+        <v>271</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>272</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>272</v>
+      </c>
+      <c r="D18" s="20" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A19" s="19" t="s">
+        <v>273</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>274</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>274</v>
+      </c>
+      <c r="D19" s="20" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A20" s="19" t="s">
+        <v>275</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>276</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>277</v>
+      </c>
+      <c r="D20" s="20" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A21" s="19" t="s">
+        <v>279</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>280</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>280</v>
+      </c>
+      <c r="D21" s="20" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A22" s="19" t="s">
+        <v>282</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>283</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>284</v>
+      </c>
+      <c r="D22" s="20" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A23" s="19" t="s">
+        <v>286</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>287</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>288</v>
+      </c>
+      <c r="D23" s="20" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A24" s="19" t="s">
+        <v>290</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>242</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>291</v>
+      </c>
+      <c r="D24" s="20" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A25" s="19" t="s">
+        <v>293</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>295</v>
+      </c>
+      <c r="D25" s="20" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A26" s="19" t="s">
+        <v>296</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>297</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>298</v>
+      </c>
+      <c r="D26" s="20" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A27" s="19" t="s">
+        <v>300</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="D27" s="20" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A28" s="19" t="s">
+        <v>303</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>304</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>305</v>
+      </c>
+      <c r="D28" s="20" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A29" s="19" t="s">
+        <v>307</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>308</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>309</v>
+      </c>
+      <c r="D29" s="20" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A30" s="19" t="s">
+        <v>310</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>280</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>280</v>
+      </c>
+      <c r="D30" s="20" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A31" s="19" t="s">
+        <v>312</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>313</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>314</v>
+      </c>
+      <c r="D31" s="20" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A32" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>315</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>316</v>
+      </c>
+      <c r="D32" s="20" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A33" s="19" t="s">
+        <v>318</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>319</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>320</v>
+      </c>
+      <c r="D33" s="20" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A34" s="19" t="s">
+        <v>322</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>323</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>324</v>
+      </c>
+      <c r="D34" s="20" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A35" s="19" t="s">
+        <v>326</v>
+      </c>
+      <c r="B35" s="6" t="s">
+        <v>327</v>
+      </c>
+      <c r="C35" s="6" t="s">
+        <v>328</v>
+      </c>
+      <c r="D35" s="21" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A36" s="19" t="s">
+        <v>330</v>
+      </c>
+      <c r="B36" s="6" t="s">
+        <v>331</v>
+      </c>
+      <c r="C36" s="6" t="s">
+        <v>332</v>
+      </c>
+      <c r="D36" s="21" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="28.9" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A37" s="22" t="s">
+        <v>334</v>
+      </c>
+      <c r="B37" s="23" t="s">
+        <v>335</v>
+      </c>
+      <c r="C37" s="23" t="s">
+        <v>336</v>
+      </c>
+      <c r="D37" s="24" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A39" s="7" t="s">
+        <v>338</v>
+      </c>
+      <c r="B39" s="8"/>
+      <c r="C39" s="9"/>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A40" s="10"/>
+      <c r="B40" s="5"/>
+      <c r="C40" s="11"/>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A41" s="10"/>
+      <c r="B41" s="5"/>
+      <c r="C41" s="11"/>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A42" s="10"/>
+      <c r="B42" s="5"/>
+      <c r="C42" s="11"/>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A43" s="10"/>
+      <c r="B43" s="5"/>
+      <c r="C43" s="11"/>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A44" s="10"/>
+      <c r="B44" s="5"/>
+      <c r="C44" s="11"/>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A45" s="10"/>
+      <c r="B45" s="5"/>
+      <c r="C45" s="11"/>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A46" s="10"/>
+      <c r="B46" s="5"/>
+      <c r="C46" s="11"/>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A47" s="10"/>
+      <c r="B47" s="5"/>
+      <c r="C47" s="11"/>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A48" s="10"/>
+      <c r="B48" s="5"/>
+      <c r="C48" s="11"/>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A49" s="10"/>
+      <c r="B49" s="5"/>
+      <c r="C49" s="11"/>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A50" s="10"/>
+      <c r="B50" s="5"/>
+      <c r="C50" s="11"/>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A51" s="10"/>
+      <c r="B51" s="5"/>
+      <c r="C51" s="11"/>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A52" s="10"/>
+      <c r="B52" s="5"/>
+      <c r="C52" s="11"/>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A53" s="10"/>
+      <c r="B53" s="5"/>
+      <c r="C53" s="11"/>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A54" s="10"/>
+      <c r="B54" s="5"/>
+      <c r="C54" s="11"/>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A55" s="10"/>
+      <c r="B55" s="5"/>
+      <c r="C55" s="11"/>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A56" s="10"/>
+      <c r="B56" s="5"/>
+      <c r="C56" s="11"/>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A57" s="10"/>
+      <c r="B57" s="5"/>
+      <c r="C57" s="11"/>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A58" s="10"/>
+      <c r="B58" s="5"/>
+      <c r="C58" s="11"/>
+    </row>
+    <row r="59" spans="1:3" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A59" s="12"/>
+      <c r="B59" s="13"/>
+      <c r="C59" s="14"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A39:C59"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>